<commit_message>
Excel good to go
</commit_message>
<xml_diff>
--- a/UnitTestProject2/02_PageObjectsAndFeatures/02_DataSheet/DataTable.xlsx
+++ b/UnitTestProject2/02_PageObjectsAndFeatures/02_DataSheet/DataTable.xlsx
@@ -16,21 +16,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>RUN_ROW</t>
   </si>
   <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
     <t>PRICE</t>
   </si>
   <si>
     <t>STATUS</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>ACCOUNT</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>98Z</t>
+  </si>
+  <si>
+    <t>24A</t>
+  </si>
+  <si>
+    <t>97Z</t>
+  </si>
+  <si>
+    <t>72R</t>
   </si>
 </sst>
 </file>
@@ -369,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,16 +400,60 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>